<commit_message>
adding 1996-2005 data; noting data errors in source document
</commit_message>
<xml_diff>
--- a/derived/county-valuation/1995b.xlsx
+++ b/derived/county-valuation/1995b.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="336">
   <si>
     <t xml:space="preserve"> Kiowa</t>
   </si>
@@ -917,7 +923,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve"> 2,713,380</t>
   </si>
   <si>
     <t xml:space="preserve">  
@@ -935,18 +941,12 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve"> 15,544,200</t>
+  </si>
+  <si>
     <t xml:space="preserve">  
 6,378,600 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,713,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> o</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 15,544,200</t>
   </si>
   <si>
     <t xml:space="preserve"> 63,136,310</t>
@@ -1049,13 +1049,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1067,7 +1085,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -1075,56 +1093,92 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="1f497d"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="eeece1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -1132,1498 +1186,1439 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="H1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="I3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="0" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="H8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="H8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="H9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="H9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="0" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="H10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="H11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="H11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="H13" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="H13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="0" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="H14" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="0" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="I15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="0" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="H16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="H16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="0" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="H17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="H17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="0" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="I19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="I19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="0" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="I20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="I20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="0" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="H21" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="0" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="H22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="0" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="H23" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="H23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="0" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="H25" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="H25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="0" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="H26" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="0" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="H27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="H27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="0" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="H28" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="H28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="H29" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="H29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
+    <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="H31" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="H31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="0" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="H33" t="s">
-        <v>4</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="H33" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="H34" t="s">
-        <v>4</v>
-      </c>
-      <c r="I34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="H34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="0" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="I35" t="s">
-        <v>4</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="I35" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="0" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
+    <row r="36" s="2" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="H36" t="s">
-        <v>298</v>
-      </c>
-      <c r="I36" t="s">
-        <v>298</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="H36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="K36" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="D37" t="s">
+      <c r="J36" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="H37" t="s">
+      <c r="K36" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="I37" t="s">
+    </row>
+    <row r="37" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="J37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="K37" t="s">
+      <c r="B38" s="0" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+      <c r="C38" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="F38" t="s">
+      <c r="H38" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="G38" t="s">
+      <c r="J38" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="H38" t="s">
-        <v>4</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="K38" s="0" t="s">
         <v>314</v>
       </c>
-      <c r="J38" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="K38" t="s">
+      <c r="B39" s="0" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
+      <c r="C39" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="F39" t="s">
+      <c r="H39" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="G39" t="s">
+      <c r="J39" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="H39" t="s">
-        <v>4</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="K39" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="J39" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="K39" t="s">
+      <c r="B40" s="0" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" t="s">
+      <c r="C40" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="G40" t="s">
+      <c r="I40" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="H40" t="s">
+      <c r="J40" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="I40" t="s">
+      <c r="K40" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="J40" t="s">
-        <v>336</v>
-      </c>
-      <c r="K40" t="s">
-        <v>337</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="5">
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A18:K18"/>
     <mergeCell ref="A24:K24"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="J36:J37"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>